<commit_message>
implement SheetCellName, SheetCellRange, SheetColumnRange
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/v0.6/XLSX/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/v0.6/XLSX/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FA6A21-28DA-1647-A85B-30F73601BA2F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2B17B4-AE18-3B40-9496-5CA3D6153068}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,12 @@
     <sheet name="table7" sheetId="9" r:id="rId9"/>
     <sheet name="lookup" sheetId="10" r:id="rId10"/>
     <sheet name="header_error" sheetId="11" r:id="rId11"/>
+    <sheet name="named_ranges" sheetId="12" r:id="rId12"/>
   </sheets>
+  <definedNames>
+    <definedName name="RANGE_B4C5">named_ranges!$B$4:$C$5</definedName>
+    <definedName name="SINGLE_CELL">named_ranges!$A$2</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>text</t>
   </si>
@@ -182,6 +187,12 @@
   </si>
   <si>
     <t>there</t>
+  </si>
+  <si>
+    <t>single cell A2</t>
+  </si>
+  <si>
+    <t>range B4:C5</t>
   </si>
 </sst>
 </file>
@@ -728,6 +739,43 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55153CDE-D96C-C844-B236-B6F5C9CAC3BD}">
+  <dimension ref="A2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F6"/>

</xml_diff>

<commit_message>
Support for local worksheet names and constants (#18)
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/v0.6/XLSX/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2B17B4-AE18-3B40-9496-5CA3D6153068}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30EE518-1D86-DE46-A38F-D231A7EA59F1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,9 +24,22 @@
     <sheet name="table7" sheetId="9" r:id="rId9"/>
     <sheet name="lookup" sheetId="10" r:id="rId10"/>
     <sheet name="header_error" sheetId="11" r:id="rId11"/>
-    <sheet name="named_ranges" sheetId="12" r:id="rId12"/>
+    <sheet name="named_ranges_2" sheetId="13" r:id="rId12"/>
+    <sheet name="named_ranges" sheetId="12" r:id="rId13"/>
   </sheets>
   <definedNames>
+    <definedName name="CONST_DATE">43383</definedName>
+    <definedName name="CONST_FLOAT">10.2</definedName>
+    <definedName name="CONST_INT">100</definedName>
+    <definedName name="CONST_LOCAL_INT" localSheetId="12">100</definedName>
+    <definedName name="CONST_LOCAL_INT">100</definedName>
+    <definedName name="LOCAL_INT" localSheetId="12">1000</definedName>
+    <definedName name="LOCAL_INT" localSheetId="11">2000</definedName>
+    <definedName name="LOCAL_INT">2000</definedName>
+    <definedName name="LOCAL_NAME" localSheetId="12">"Hey You"</definedName>
+    <definedName name="LOCAL_NAME" localSheetId="11">"out there in the cold"</definedName>
+    <definedName name="LOCAL_NAME">"out there in the cold"</definedName>
+    <definedName name="out_there_in_the_cold">named_ranges_2!$A$2</definedName>
     <definedName name="RANGE_B4C5">named_ranges!$B$4:$C$5</definedName>
     <definedName name="SINGLE_CELL">named_ranges!$A$2</definedName>
   </definedNames>
@@ -43,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>text</t>
   </si>
@@ -193,6 +206,12 @@
   </si>
   <si>
     <t>range B4:C5</t>
+  </si>
+  <si>
+    <t>local name</t>
+  </si>
+  <si>
+    <t>float cient</t>
   </si>
 </sst>
 </file>
@@ -228,12 +247,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,6 +591,14 @@
       </c>
       <c r="B6" s="3">
         <v>43206.805447106482</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="5">
+        <v>-220</v>
       </c>
     </row>
   </sheetData>
@@ -740,10 +768,43 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55153CDE-D96C-C844-B236-B6F5C9CAC3BD}">
-  <dimension ref="A2:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF9316C-B24C-5844-B9B5-93022A9927D0}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="str">
+        <f>LOCAL_NAME</f>
+        <v>out there in the cold</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f>CONST_INT</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>LOCAL_INT</f>
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55153CDE-D96C-C844-B236-B6F5C9CAC3BD}">
+  <dimension ref="A2:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -769,6 +830,35 @@
       </c>
       <c r="C5" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <f>CONST_INT</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>LOCAL_NAME</f>
+        <v>Hey You</v>
+      </c>
+      <c r="B9">
+        <f>CONST_DATE</f>
+        <v>43383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f>LOCAL_INT</f>
+        <v>1000</v>
+      </c>
+      <c r="B10">
+        <f>CONST_FLOAT</f>
+        <v>10.199999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix parsing of local definedNames
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/v0.6/XLSX/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30EE518-1D86-DE46-A38F-D231A7EA59F1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06093FED-236D-114C-903C-DC6238C1EA8B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,8 @@
     <definedName name="LOCAL_NAME" localSheetId="12">"Hey You"</definedName>
     <definedName name="LOCAL_NAME" localSheetId="11">"out there in the cold"</definedName>
     <definedName name="LOCAL_NAME">"out there in the cold"</definedName>
+    <definedName name="LOCAL_REF" localSheetId="12">named_ranges!$A$15:$B$15</definedName>
+    <definedName name="LOCAL_REF" localSheetId="11">named_ranges_2!$D$1:$E$1</definedName>
     <definedName name="out_there_in_the_cold">named_ranges_2!$A$2</definedName>
     <definedName name="RANGE_B4C5">named_ranges!$B$4:$C$5</definedName>
     <definedName name="SINGLE_CELL">named_ranges!$A$2</definedName>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
   <si>
     <t>text</t>
   </si>
@@ -212,6 +214,12 @@
   </si>
   <si>
     <t>float cient</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>reference</t>
   </si>
 </sst>
 </file>
@@ -536,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -769,30 +777,48 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF9316C-B24C-5844-B9B5-93022A9927D0}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>LOCAL_NAME</f>
         <v>out there in the cold</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>CONST_INT</f>
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>LOCAL_INT</f>
         <v>2000</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="str">
+        <f>LOCAL_REF</f>
+        <v>local</v>
+      </c>
+      <c r="E4" t="str">
+        <f>LOCAL_REF</f>
+        <v>reference</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -800,10 +826,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55153CDE-D96C-C844-B236-B6F5C9CAC3BD}">
-  <dimension ref="A2:C10"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,12 +837,19 @@
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <f t="array" ref="E2:F2">LOCAL_REF</f>
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -824,7 +857,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>49</v>
       </c>
@@ -832,7 +865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -841,7 +874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>LOCAL_NAME</f>
         <v>Hey You</v>
@@ -851,7 +884,7 @@
         <v>43383</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>LOCAL_INT</f>
         <v>1000</v>
@@ -859,6 +892,14 @@
       <c r="B10">
         <f>CONST_FLOAT</f>
         <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix regex for integers
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/v0.6/XLSX/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06093FED-236D-114C-903C-DC6238C1EA8B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB9556-48F5-C545-8F22-191D0EBD4DE8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>text</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>reference</t>
+  </si>
+  <si>
+    <t>integer neg</t>
+  </si>
+  <si>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>bigint neg</t>
   </si>
 </sst>
 </file>
@@ -542,15 +551,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -607,6 +616,31 @@
       </c>
       <c r="B7" s="5">
         <v>-220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>100000000000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <f>-100000000000000</f>
+        <v>-100000000000000</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF9316C-B24C-5844-B9B5-93022A9927D0}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
User friendly workaround when trying to get collumns label with badly done table header (#164)
* Add defalut behavior on column with problematic labels
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/v0.6/XLSX/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BC5234\Documents\Julia\XLSX\XLSX.jl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB9556-48F5-C545-8F22-191D0EBD4DE8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4656FDE3-A054-4CC4-B7F3-D43EFC541B39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="3000" windowWidth="28800" windowHeight="15435" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,16 @@
     <definedName name="RANGE_B4C5">named_ranges!$B$4:$C$5</definedName>
     <definedName name="SINGLE_CELL">named_ranges!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>text</t>
   </si>
@@ -229,6 +235,12 @@
   </si>
   <si>
     <t>bigint neg</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>now</t>
   </si>
 </sst>
 </file>
@@ -553,16 +565,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -578,7 +590,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -586,7 +598,7 @@
         <v>102.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -594,7 +606,7 @@
         <v>30422</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -602,7 +614,7 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -610,7 +622,7 @@
         <v>43206.805447106482</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -618,7 +630,7 @@
         <v>-220</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -626,7 +638,7 @@
         <v>-2000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -634,7 +646,7 @@
         <v>100000000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -656,9 +668,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>37</v>
       </c>
@@ -681,7 +693,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>10</v>
       </c>
@@ -706,7 +718,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>20</v>
       </c>
@@ -731,7 +743,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>30</v>
       </c>
@@ -763,15 +775,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2122C239-B27E-4F47-96FD-DE9E78741957}">
-  <dimension ref="B2:D4"/>
+  <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>43</v>
       </c>
@@ -782,7 +792,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>10</v>
       </c>
@@ -792,8 +802,11 @@
       <c r="D3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>20</v>
       </c>
@@ -802,6 +815,9 @@
       </c>
       <c r="D4" t="s">
         <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -817,9 +833,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>LOCAL_NAME</f>
         <v>out there in the cold</v>
@@ -831,19 +847,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>CONST_INT</f>
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>LOCAL_INT</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" t="str">
         <f>LOCAL_REF</f>
         <v>local</v>
@@ -866,12 +882,12 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -883,7 +899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -891,7 +907,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>49</v>
       </c>
@@ -899,7 +915,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -908,7 +924,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>LOCAL_NAME</f>
         <v>Hey You</v>
@@ -918,7 +934,7 @@
         <v>43383</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>LOCAL_INT</f>
         <v>1000</v>
@@ -928,7 +944,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -949,9 +965,9 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -965,17 +981,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -986,7 +1002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1007,9 +1023,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>29</v>
       </c>
@@ -1020,17 +1036,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>34</v>
       </c>
@@ -1048,9 +1064,9 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1086,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1084,7 +1100,7 @@
         <v>0.20011323191065111</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -1103,7 +1119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1122,7 +1138,7 @@
         <v>9.5059167683513524E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1144,7 +1160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1160,7 +1176,7 @@
         <v>0.82422780912015003</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -1182,7 +1198,7 @@
         <v>0.62058835778747101</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1201,7 +1217,7 @@
         <v>0.91741510177329644</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1223,7 +1239,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1243,7 +1259,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
         <v>11</v>
       </c>
@@ -1261,9 +1277,9 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1274,7 +1290,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1282,7 +1298,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1290,12 +1306,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
@@ -1313,7 +1329,7 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1327,34 +1343,34 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>5</v>
       </c>
@@ -1372,39 +1388,39 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>5</v>
       </c>
@@ -1422,39 +1438,39 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added a setFormat function (no tests yet)
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BC5234\Documents\Julia\XLSX\XLSX.jl\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4656FDE3-A054-4CC4-B7F3-D43EFC541B39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{4656FDE3-A054-4CC4-B7F3-D43EFC541B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53EABF5C-0BD1-4A68-B617-EDDAA3894199}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="3000" windowWidth="28800" windowHeight="15435" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -276,13 +281,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,18 +569,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -590,23 +596,25 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>102.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>30422</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -614,7 +622,7 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -622,7 +630,7 @@
         <v>43206.805447106482</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -630,7 +638,7 @@
         <v>-220</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -638,7 +646,7 @@
         <v>-2000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -646,7 +654,7 @@
         <v>100000000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -668,7 +676,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -777,9 +785,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2122C239-B27E-4F47-96FD-DE9E78741957}">
   <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -833,7 +841,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
@@ -882,7 +890,7 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.625" customWidth="1"/>
   </cols>
@@ -965,7 +973,7 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1023,7 +1031,7 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="12" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
@@ -1064,7 +1072,7 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1277,7 +1285,7 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1329,7 +1337,7 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1343,7 +1351,7 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -1388,7 +1396,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -1438,7 +1446,7 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2">

</xml_diff>

<commit_message>
Minor row range fixes
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{4656FDE3-A054-4CC4-B7F3-D43EFC541B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53EABF5C-0BD1-4A68-B617-EDDAA3894199}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{4656FDE3-A054-4CC4-B7F3-D43EFC541B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB6D7060-29A3-4BA5-BF86-684715D6DE7E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -252,10 +252,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -571,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -672,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -731,11 +737,11 @@
         <v>20</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C5" si="0">VLOOKUP(B4,$F$3:$G$5,2,FALSE)</f>
+        <f t="shared" ref="C4:C6" si="0">VLOOKUP(B4,$F$3:$G$5,2,FALSE)</f>
         <v>name2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D5" si="1">VLOOKUP(B4,$I$3:$J$5,2,FALSE)</f>
+        <f t="shared" ref="D4:D9" si="1">VLOOKUP(B4,$I$3:$J$5,2,FALSE)</f>
         <v>200</v>
       </c>
       <c r="F4">
@@ -777,6 +783,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adding tests to improve code coverage
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{4656FDE3-A054-4CC4-B7F3-D43EFC541B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB6D7060-29A3-4BA5-BF86-684715D6DE7E}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{4656FDE3-A054-4CC4-B7F3-D43EFC541B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E47BC31F-2FC6-4085-9BE7-B6682648EB1F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -310,6 +310,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,13 +581,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -678,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:J5"/>
     </sheetView>
   </sheetViews>
@@ -737,11 +741,11 @@
         <v>20</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C6" si="0">VLOOKUP(B4,$F$3:$G$5,2,FALSE)</f>
+        <f t="shared" ref="C4:C5" si="0">VLOOKUP(B4,$F$3:$G$5,2,FALSE)</f>
         <v>name2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" si="1">VLOOKUP(B4,$I$3:$J$5,2,FALSE)</f>
+        <f t="shared" ref="D4:D5" si="1">VLOOKUP(B4,$I$3:$J$5,2,FALSE)</f>
         <v>200</v>
       </c>
       <c r="F4">

</xml_diff>

<commit_message>
Fix #312 and update to XML.jl 0.3.6 to fix #303
</commit_message>
<xml_diff>
--- a/data/general.xlsx
+++ b/data/general.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{4656FDE3-A054-4CC4-B7F3-D43EFC541B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E47BC31F-2FC6-4085-9BE7-B6682648EB1F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -310,10 +310,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -581,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1079,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>